<commit_message>
Update 1 oktober 2021
</commit_message>
<xml_diff>
--- a/data_psak.xlsx
+++ b/data_psak.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Pro-Psak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D122A6DA-7E0D-49E1-BADC-14B7FBEB8EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C352A14A-AFE5-4AD5-A3BF-B9AE8BDDD550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>No</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Pend Fidusia</t>
-  </si>
-  <si>
-    <t>Pend Provisi</t>
   </si>
   <si>
     <t>ACTIVE</t>
@@ -821,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -849,10 +846,9 @@
     <col min="18" max="18" width="12" style="6" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7265625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,10 +862,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -913,37 +909,34 @@
       <c r="T1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="J2" s="7">
         <v>35</v>
@@ -952,7 +945,7 @@
         <v>23</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="9">
         <v>0</v>
@@ -978,37 +971,34 @@
       <c r="T2" s="9">
         <v>0</v>
       </c>
-      <c r="U2" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="J3" s="7">
         <v>34</v>
@@ -1017,7 +1007,7 @@
         <v>27</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="9">
         <v>1172378</v>
@@ -1043,37 +1033,34 @@
       <c r="T3" s="9">
         <v>0</v>
       </c>
-      <c r="U3" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="J4" s="7">
         <v>21</v>
@@ -1082,7 +1069,7 @@
         <v>26</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="9">
         <v>1448106</v>
@@ -1108,37 +1095,34 @@
       <c r="T4" s="9">
         <v>0</v>
       </c>
-      <c r="U4" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="J5" s="7">
         <v>27</v>
@@ -1147,7 +1131,7 @@
         <v>24</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M5" s="9">
         <v>1084042</v>
@@ -1173,37 +1157,34 @@
       <c r="T5" s="9">
         <v>0</v>
       </c>
-      <c r="U5" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="J6" s="7">
         <v>15</v>
@@ -1212,7 +1193,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" s="9">
         <v>203508</v>
@@ -1238,37 +1219,34 @@
       <c r="T6" s="9">
         <v>0</v>
       </c>
-      <c r="U6" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="J7" s="7">
         <v>23</v>
@@ -1277,7 +1255,7 @@
         <v>25</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="9">
         <v>544241</v>
@@ -1303,37 +1281,34 @@
       <c r="T7" s="9">
         <v>0</v>
       </c>
-      <c r="U7" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="J8" s="7">
         <v>19</v>
@@ -1342,7 +1317,7 @@
         <v>23</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M8" s="9">
         <v>68162</v>
@@ -1368,37 +1343,34 @@
       <c r="T8" s="9">
         <v>0</v>
       </c>
-      <c r="U8" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="J9" s="7">
         <v>16</v>
@@ -1407,7 +1379,7 @@
         <v>26</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M9" s="9">
         <v>0</v>
@@ -1433,37 +1405,34 @@
       <c r="T9" s="9">
         <v>0</v>
       </c>
-      <c r="U9" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="I10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="7">
         <v>17</v>
@@ -1472,7 +1441,7 @@
         <v>24</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M10" s="9">
         <v>0</v>
@@ -1498,37 +1467,34 @@
       <c r="T10" s="9">
         <v>0</v>
       </c>
-      <c r="U10" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="J11" s="7">
         <v>12</v>
@@ -1537,7 +1503,7 @@
         <v>24</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M11" s="9">
         <v>49694</v>
@@ -1563,37 +1529,34 @@
       <c r="T11" s="9">
         <v>0</v>
       </c>
-      <c r="U11" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="I12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="7">
         <v>51</v>
@@ -1602,7 +1565,7 @@
         <v>24</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M12" s="9">
         <v>2510524</v>
@@ -1628,37 +1591,34 @@
       <c r="T12" s="9">
         <v>0</v>
       </c>
-      <c r="U12" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="J13" s="7">
         <v>50</v>
@@ -1667,7 +1627,7 @@
         <v>31</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M13" s="9">
         <v>11379096</v>
@@ -1693,37 +1653,34 @@
       <c r="T13" s="9">
         <v>0</v>
       </c>
-      <c r="U13" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="J14" s="7">
         <v>8</v>
@@ -1732,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M14" s="9">
         <v>49739</v>
@@ -1758,37 +1715,34 @@
       <c r="T14" s="9">
         <v>0</v>
       </c>
-      <c r="U14" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="J15" s="7">
         <v>35</v>
@@ -1797,7 +1751,7 @@
         <v>17</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M15" s="9">
         <v>2990995</v>
@@ -1823,37 +1777,34 @@
       <c r="T15" s="9">
         <v>0</v>
       </c>
-      <c r="U15" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="J16" s="7">
         <v>37</v>
@@ -1862,7 +1813,7 @@
         <v>10</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M16" s="9">
         <v>3478406</v>
@@ -1888,11 +1839,8 @@
       <c r="T16" s="9">
         <v>0</v>
       </c>
-      <c r="U16" s="9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1913,7 +1861,6 @@
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">

</xml_diff>